<commit_message>
Improve Excel exporter to create new sheets for new years
</commit_message>
<xml_diff>
--- a/test/data/sample1.xlsx
+++ b/test/data/sample1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mme/dev/worktimer/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4C6EBB7-B110-1641-B1E1-A87E4CE7C8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9664B619-571C-D847-8674-FBB1403FAC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18440" yWindow="500" windowWidth="32760" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="2021" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -133,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Eintragung erfolgt in min</t>
   </si>
@@ -208,6 +207,21 @@
   </si>
   <si>
     <t>doc</t>
+  </si>
+  <si>
+    <t>adm</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>sup</t>
+  </si>
+  <si>
+    <t>Support</t>
   </si>
 </sst>
 </file>
@@ -791,7 +805,7 @@
   <dimension ref="A1:BL25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -861,7 +875,7 @@
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:O3" si="0">CONCATENATE(TEXT(INT(D4/60),0),":",TEXT(MOD(D4,60),"00"))</f>
-        <v>184:36</v>
+        <v>166:39</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -916,7 +930,7 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ref="D4:O4" si="1">SUM(D5:D27)</f>
-        <v>11076</v>
+        <v>9999</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="1"/>
@@ -987,9 +1001,7 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6">
-        <v>897</v>
-      </c>
+      <c r="D6"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
@@ -1001,9 +1013,7 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7">
-        <v>180</v>
-      </c>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
@@ -1014,6 +1024,28 @@
       </c>
       <c r="C8" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:11">

</xml_diff>